<commit_message>
Changes to be committed: 	modified:   backtest/bt_grid/backtest_report/grid_result.png 	modified:   backtest/bt_grid/backtest_report/portfolio.csv 	modified:   backtest/bt_grid/backtest_report/stock_account.csv 	modified:   backtest/bt_grid/backtest_report/stock_positions.csv 	modified:   backtest/bt_grid/backtest_report/summary.xlsx 	modified:   backtest/bt_grid/backtest_report/trades.csv 	modified:   backtest/bt_grid/bt_grid.py
</commit_message>
<xml_diff>
--- a/backtest/bt_grid/backtest_report/summary.xlsx
+++ b/backtest/bt_grid/backtest_report/summary.xlsx
@@ -617,7 +617,7 @@
       </c>
       <c r="B2" s="5" t="inlineStr">
         <is>
-          <t>2013-01-04</t>
+          <t>2016-09-30</t>
         </is>
       </c>
       <c r="C2" s="13" t="n"/>
@@ -633,7 +633,7 @@
       </c>
       <c r="B3" s="5" t="inlineStr">
         <is>
-          <t>2020-12-31</t>
+          <t>2022-07-01</t>
         </is>
       </c>
       <c r="C3" s="13" t="n"/>
@@ -665,7 +665,7 @@
       </c>
       <c r="B5" s="5" t="inlineStr">
         <is>
-          <t>STOCK:10000000.0</t>
+          <t>STOCK:1000000.0</t>
         </is>
       </c>
       <c r="C5" s="13" t="n"/>
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="B8" s="7" t="n">
-        <v>31446384.7941239</v>
+        <v>984027.4138720001</v>
       </c>
       <c r="C8" s="13" t="n"/>
       <c r="D8" s="13" t="n"/>
@@ -726,7 +726,7 @@
         </is>
       </c>
       <c r="B9" s="7" t="n">
-        <v>8475696.006923905</v>
+        <v>700038.713872</v>
       </c>
       <c r="C9" s="13" t="n"/>
       <c r="D9" s="13" t="n"/>
@@ -740,7 +740,7 @@
         </is>
       </c>
       <c r="B10" s="7" t="n">
-        <v>2.14463847941239</v>
+        <v>-0.0159725861279999</v>
       </c>
       <c r="C10" s="13" t="n"/>
       <c r="D10" s="13" t="n"/>
@@ -754,7 +754,7 @@
         </is>
       </c>
       <c r="B11" s="7" t="n">
-        <v>0.1600233917228855</v>
+        <v>-0.002902358584843112</v>
       </c>
       <c r="C11" s="13" t="n"/>
       <c r="D11" s="13" t="n"/>
@@ -768,7 +768,7 @@
         </is>
       </c>
       <c r="B12" s="7" t="n">
-        <v>3.14463847941239</v>
+        <v>0.9840274138720001</v>
       </c>
       <c r="C12" s="13" t="n"/>
       <c r="D12" s="13" t="n"/>
@@ -782,7 +782,7 @@
         </is>
       </c>
       <c r="B13" s="7" t="n">
-        <v>10000000</v>
+        <v>1000000</v>
       </c>
       <c r="C13" s="13" t="n"/>
       <c r="D13" s="13" t="n"/>
@@ -796,7 +796,7 @@
         </is>
       </c>
       <c r="B14" s="7" t="n">
-        <v>1.299002994101257</v>
+        <v>0.506763355378131</v>
       </c>
       <c r="C14" s="13" t="n"/>
       <c r="D14" s="13" t="n"/>
@@ -810,7 +810,7 @@
         </is>
       </c>
       <c r="B15" s="7" t="n">
-        <v>0.02369121258148804</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="16" ht="20" customHeight="1">
@@ -820,7 +820,7 @@
         </is>
       </c>
       <c r="B16" s="5" t="n">
-        <v>0.2275912518284239</v>
+        <v>0.08896021722647571</v>
       </c>
       <c r="C16" s="13" t="n"/>
       <c r="D16" s="13" t="n"/>
@@ -834,7 +834,7 @@
         </is>
       </c>
       <c r="B17" s="5" t="n">
-        <v>0.6153146419226194</v>
+        <v>-0.2712562787819109</v>
       </c>
       <c r="C17" s="13" t="n"/>
       <c r="D17" s="13" t="n"/>
@@ -848,7 +848,7 @@
         </is>
       </c>
       <c r="B18" s="5" t="n">
-        <v>0.1670806931737925</v>
+        <v>0.0592497017799764</v>
       </c>
       <c r="C18" s="13" t="n"/>
       <c r="D18" s="13" t="n"/>
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="B19" s="5" t="n">
-        <v>0.8381592568440059</v>
+        <v>-0.407276606624869</v>
       </c>
       <c r="C19" s="13" t="n"/>
       <c r="D19" s="13" t="n"/>
@@ -876,7 +876,7 @@
         </is>
       </c>
       <c r="B20" s="5" t="n">
-        <v>0.5555567276017497</v>
+        <v>0.147618593250995</v>
       </c>
       <c r="C20" s="13" t="n"/>
       <c r="D20" s="13" t="n"/>
@@ -890,7 +890,7 @@
         </is>
       </c>
       <c r="B21" s="5" t="n">
-        <v>0.02332280539487548</v>
+        <v>0.009255177447469523</v>
       </c>
       <c r="C21" s="13" t="n"/>
       <c r="D21" s="13" t="n"/>
@@ -904,7 +904,7 @@
         </is>
       </c>
       <c r="B22" s="7" t="n">
-        <v>-0.3946803338322213</v>
+        <v>-0.4440485719580742</v>
       </c>
       <c r="C22" s="13" t="n"/>
       <c r="D22" s="13" t="n"/>
@@ -918,7 +918,7 @@
         </is>
       </c>
       <c r="B23" s="7" t="n">
-        <v>-0.06297042510195849</v>
+        <v>-0.1005539199401437</v>
       </c>
       <c r="C23" s="13" t="n"/>
       <c r="D23" s="13" t="n"/>
@@ -932,7 +932,7 @@
         </is>
       </c>
       <c r="B24" s="7" t="n">
-        <v>0.005012753380233437</v>
+        <v>-0.03306533688864361</v>
       </c>
       <c r="C24" s="13" t="n"/>
       <c r="D24" s="13" t="n"/>
@@ -946,7 +946,7 @@
         </is>
       </c>
       <c r="B25" s="7" t="n">
-        <v>0.7157018927787725</v>
+        <v>0.2080889540572083</v>
       </c>
       <c r="C25" s="13" t="n"/>
       <c r="D25" s="13" t="n"/>
@@ -960,7 +960,7 @@
         </is>
       </c>
       <c r="B26" s="7" t="n">
-        <v>2.010391538108703</v>
+        <v>-0.1850583140636529</v>
       </c>
       <c r="C26" s="13" t="n"/>
       <c r="D26" s="13" t="n"/>
@@ -974,7 +974,7 @@
         </is>
       </c>
       <c r="B27" s="7" t="n">
-        <v>-0.672049906663543</v>
+        <v>-0.3662156100920644</v>
       </c>
       <c r="C27" s="13" t="n"/>
       <c r="D27" s="13" t="n"/>
@@ -988,7 +988,7 @@
         </is>
       </c>
       <c r="B28" s="7" t="n">
-        <v>0.4017448221708894</v>
+        <v>0.679665020136522</v>
       </c>
       <c r="C28" s="13" t="n"/>
       <c r="D28" s="13" t="n"/>
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="B29" s="7" t="n">
-        <v>0.09066397195748703</v>
+        <v>0.2220371545660234</v>
       </c>
       <c r="C29" s="13" t="n"/>
       <c r="D29" s="13" t="n"/>
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="B30" s="5" t="n">
-        <v>0.004747815913053399</v>
+        <v>-0.03249006312204741</v>
       </c>
       <c r="C30" s="13" t="n"/>
       <c r="D30" s="13" t="n"/>
@@ -1030,7 +1030,7 @@
         </is>
       </c>
       <c r="B31" s="5" t="n">
-        <v>0.7153971483258268</v>
+        <v>0.1955501287967914</v>
       </c>
       <c r="C31" s="13" t="n"/>
       <c r="D31" s="13" t="n"/>
@@ -1044,7 +1044,7 @@
         </is>
       </c>
       <c r="B32" s="5" t="n">
-        <v>0.6224041583292651</v>
+        <v>-0.2954046612898738</v>
       </c>
       <c r="C32" s="13" t="n"/>
       <c r="D32" s="13" t="n"/>
@@ -1058,7 +1058,7 @@
         </is>
       </c>
       <c r="B33" s="5" t="n">
-        <v>0.845025178889058</v>
+        <v>-0.4474291894205973</v>
       </c>
     </row>
     <row r="34" ht="20" customHeight="1">
@@ -1068,7 +1068,7 @@
         </is>
       </c>
       <c r="B34" s="5" t="n">
-        <v>2.05206416811407</v>
+        <v>-0.1779767705087284</v>
       </c>
     </row>
     <row r="35" ht="20" customHeight="1">
@@ -1078,7 +1078,7 @@
         </is>
       </c>
       <c r="B35" s="5" t="n">
-        <v>0.01191090647596943</v>
+        <v>0.02940989152393217</v>
       </c>
     </row>
     <row r="36" ht="20" customHeight="1">
@@ -1088,7 +1088,7 @@
         </is>
       </c>
       <c r="B36" s="16" t="n">
-        <v>0.5379598052987522</v>
+        <v>0.1425394589588236</v>
       </c>
     </row>
   </sheetData>
@@ -1102,7 +1102,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
@@ -1154,162 +1154,142 @@
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="9" t="n">
-        <v>2013</v>
+        <v>2016</v>
       </c>
       <c r="B2" s="13" t="n">
-        <v>0.6137820000000003</v>
+        <v>0.002901000000000506</v>
       </c>
       <c r="C2" s="13" t="n">
-        <v>-0.137771099550383</v>
+        <v>0.09083838214307459</v>
       </c>
       <c r="D2" s="13" t="n">
-        <v>2.135063851546433</v>
+        <v>-0.1168510312431997</v>
       </c>
       <c r="E2" s="13" t="n">
-        <v>-0.7329009628764058</v>
+        <v>1.517732139280756</v>
       </c>
       <c r="F2" s="13" t="n">
-        <v>0.4038461538461539</v>
+        <v>0.7692307692307693</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="9" t="n">
-        <v>2014</v>
+        <v>2017</v>
       </c>
       <c r="B3" s="13" t="n">
-        <v>0.102271558364142</v>
+        <v>-0.02175987460377408</v>
       </c>
       <c r="C3" s="13" t="n">
-        <v>-0.03993796863095373</v>
+        <v>0.06988215337423431</v>
       </c>
       <c r="D3" s="13" t="n">
-        <v>0.6463547471799835</v>
+        <v>-0.4223747510391208</v>
       </c>
       <c r="E3" s="13" t="n">
-        <v>3.601901604407146</v>
+        <v>-0.1989114154221593</v>
       </c>
       <c r="F3" s="13" t="n">
-        <v>0.3962264150943396</v>
+        <v>0.5294117647058824</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="9" t="n">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="B4" s="13" t="n">
-        <v>0.5796991948622299</v>
+        <v>-0.07093829440676516</v>
       </c>
       <c r="C4" s="13" t="n">
-        <v>-0.204929896759058</v>
+        <v>0.2257590709850036</v>
       </c>
       <c r="D4" s="13" t="n">
-        <v>1.505291706075436</v>
+        <v>-0.9476495755600048</v>
       </c>
       <c r="E4" s="13" t="n">
-        <v>-2.863825391002649</v>
+        <v>-0.2672593229917987</v>
       </c>
       <c r="F4" s="13" t="n">
-        <v>0.3076923076923077</v>
+        <v>0.6078431372549019</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="9" t="n">
-        <v>2016</v>
+        <v>2019</v>
       </c>
       <c r="B5" s="13" t="n">
-        <v>-0.1963220771456318</v>
+        <v>0.1045034350650915</v>
       </c>
       <c r="C5" s="13" t="n">
-        <v>0.07533711756787831</v>
+        <v>-0.2667513710070671</v>
       </c>
       <c r="D5" s="13" t="n">
-        <v>-0.8168451754510518</v>
+        <v>1.020058046290432</v>
       </c>
       <c r="E5" s="13" t="n">
-        <v>-0.2057290738979336</v>
+        <v>-0.3950745684775894</v>
       </c>
       <c r="F5" s="13" t="n">
-        <v>0.5</v>
+        <v>0.3846153846153846</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="9" t="n">
-        <v>2017</v>
+        <v>2020</v>
       </c>
       <c r="B6" s="13" t="n">
-        <v>-0.0730455913915638</v>
+        <v>0.05331293736683378</v>
       </c>
       <c r="C6" s="13" t="n">
-        <v>0.02965195180581313</v>
+        <v>-0.4046443323225831</v>
       </c>
       <c r="D6" s="13" t="n">
-        <v>-0.611026669207739</v>
+        <v>0.5025377402368426</v>
       </c>
       <c r="E6" s="13" t="n">
-        <v>1.493743664569422</v>
+        <v>-1.3498412884142</v>
       </c>
       <c r="F6" s="13" t="n">
-        <v>0.5490196078431373</v>
+        <v>0.3653846153846154</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="9" t="n">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="B7" s="13" t="n">
-        <v>-0.2117646047231722</v>
+        <v>-0.01279320110108746</v>
       </c>
       <c r="C7" s="13" t="n">
-        <v>0.08138561722599656</v>
+        <v>-0.1734313822401421</v>
       </c>
       <c r="D7" s="13" t="n">
-        <v>-1.128848856541622</v>
+        <v>-0.1258918879863881</v>
       </c>
       <c r="E7" s="13" t="n">
-        <v>-1.878989405571127</v>
+        <v>-0.4294230782910119</v>
       </c>
       <c r="F7" s="13" t="n">
-        <v>0.5490196078431373</v>
+        <v>0.3653846153846154</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="9" t="n">
-        <v>2019</v>
+        <v>2022</v>
       </c>
       <c r="B8" s="13" t="n">
-        <v>0.3172954959071599</v>
+        <v>-0.0600033816023634</v>
       </c>
       <c r="C8" s="13" t="n">
-        <v>-0.1005122847576974</v>
+        <v>0.07703172984241145</v>
       </c>
       <c r="D8" s="13" t="n">
-        <v>1.602511043443668</v>
+        <v>-1.518050989238576</v>
       </c>
       <c r="E8" s="13" t="n">
-        <v>0.05266064011291469</v>
+        <v>-1.099859491357237</v>
       </c>
       <c r="F8" s="13" t="n">
-        <v>0.4230769230769231</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="9" t="n">
-        <v>2020</v>
-      </c>
-      <c r="B9" s="13" t="n">
-        <v>0.4467158530004297</v>
-      </c>
-      <c r="C9" s="13" t="n">
-        <v>-0.1460222486864249</v>
-      </c>
-      <c r="D9" s="13" t="n">
-        <v>1.825954342949339</v>
-      </c>
-      <c r="E9" s="13" t="n">
-        <v>-8.860088704495043</v>
-      </c>
-      <c r="F9" s="13" t="n">
-        <v>0.4038461538461539</v>
+        <v>0.48</v>
       </c>
     </row>
   </sheetData>
@@ -1323,7 +1303,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A1" sqref="A1:XFD2"/>
@@ -1401,330 +1381,289 @@
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="15" t="n">
-        <v>2013</v>
+        <v>2016</v>
       </c>
       <c r="B2" s="15" t="n">
-        <v>0.08000399999999996</v>
+        <v/>
       </c>
       <c r="C2" s="15" t="n">
-        <v>0.08878022673990116</v>
+        <v/>
       </c>
       <c r="D2" s="15" t="n">
-        <v>0.004901831553541847</v>
+        <v/>
       </c>
       <c r="E2" s="15" t="n">
-        <v>0.02086233583350783</v>
+        <v/>
       </c>
       <c r="F2" s="15" t="n">
-        <v>0.1569431560727284</v>
+        <v/>
       </c>
       <c r="G2" s="15" t="n">
-        <v>-0.04285323267584962</v>
+        <v/>
       </c>
       <c r="H2" s="15" t="n">
-        <v>0.08990527894165123</v>
+        <v/>
       </c>
       <c r="I2" s="15" t="n">
-        <v>0.03270591532192157</v>
+        <v/>
       </c>
       <c r="J2" s="15" t="n">
-        <v>0.1109987090389226</v>
+        <v>-4.8000000000048e-05</v>
       </c>
       <c r="K2" s="15" t="n">
-        <v>-0.0707097192863354</v>
+        <v>0.01268160871721791</v>
       </c>
       <c r="L2" s="15" t="n">
-        <v>0.07547030031449942</v>
+        <v>0.02038547035303107</v>
       </c>
       <c r="M2" s="15" t="n">
-        <v>-0.03335032486571998</v>
+        <v>-0.02939679233815573</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="15" t="n">
-        <v>2014</v>
+        <v>2017</v>
       </c>
       <c r="B3" s="15" t="n">
-        <v>0.1045215524773482</v>
+        <v>0.004117056419327358</v>
       </c>
       <c r="C3" s="15" t="n">
-        <v>-0.02938584212690698</v>
+        <v>0.0032213538822079</v>
       </c>
       <c r="D3" s="15" t="n">
-        <v>-0.05308026574524383</v>
+        <v>-0.01050903022348382</v>
       </c>
       <c r="E3" s="15" t="n">
-        <v>-0.0227163824702652</v>
+        <v>-0.00501472004897674</v>
       </c>
       <c r="F3" s="15" t="n">
-        <v>0.01956802808192215</v>
+        <v>-0.002668291368570053</v>
       </c>
       <c r="G3" s="15" t="n">
-        <v>0.04758879633708046</v>
+        <v>0.006243006481920332</v>
       </c>
       <c r="H3" s="15" t="n">
-        <v>-0.02835487570181106</v>
+        <v>0.01299861848979611</v>
       </c>
       <c r="I3" s="15" t="n">
-        <v>0.04344008286223788</v>
+        <v>0.02158218596895867</v>
       </c>
       <c r="J3" s="15" t="n">
-        <v>0.05817107728938375</v>
+        <v>-0.004852945020285881</v>
       </c>
       <c r="K3" s="15" t="n">
-        <v>-0.01303783310003792</v>
+        <v>-0.02209018179554223</v>
       </c>
       <c r="L3" s="15" t="n">
-        <v>0.02755396497971785</v>
+        <v>0.001173825676939577</v>
       </c>
       <c r="M3" s="15" t="n">
-        <v>-0.04392772913043197</v>
+        <v>-0.0251997138428518</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="15" t="n">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="B4" s="15" t="n">
-        <v>0.09805568391736963</v>
+        <v>0.02104114045978056</v>
       </c>
       <c r="C4" s="15" t="n">
-        <v>0.1032340970177907</v>
+        <v>-0.03444372235382909</v>
       </c>
       <c r="D4" s="15" t="n">
-        <v>0.1456722657098359</v>
+        <v>-0.005182906025321787</v>
       </c>
       <c r="E4" s="15" t="n">
-        <v>0.1537216461438757</v>
+        <v>-0.003371422929625001</v>
       </c>
       <c r="F4" s="15" t="n">
-        <v>0.1659834540365714</v>
+        <v>-0.01506839172813057</v>
       </c>
       <c r="G4" s="15" t="n">
-        <v>-0.1354285352957473</v>
+        <v>-0.02404101169811712</v>
       </c>
       <c r="H4" s="15" t="n">
-        <v>-0.07650790875666236</v>
+        <v>0</v>
       </c>
       <c r="I4" s="15" t="n">
-        <v>-0.1496511772179633</v>
+        <v>-0.01119760816833082</v>
       </c>
       <c r="J4" s="15" t="n">
-        <v>0.031017206304913</v>
+        <v>0.003882687754667602</v>
       </c>
       <c r="K4" s="15" t="n">
-        <v>0.1323324519486169</v>
+        <v>0.007412944620942774</v>
       </c>
       <c r="L4" s="15" t="n">
-        <v>0.05608855219456399</v>
+        <v>0.005438249345847357</v>
       </c>
       <c r="M4" s="15" t="n">
-        <v>0.01078114759582505</v>
+        <v>-0.01654587690989706</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="15" t="n">
-        <v>2016</v>
+        <v>2019</v>
       </c>
       <c r="B5" s="15" t="n">
-        <v>-0.1909406016348695</v>
+        <v>0.01811774670262323</v>
       </c>
       <c r="C5" s="15" t="n">
-        <v>-0.03828737191907539</v>
+        <v>0.07340764399846544</v>
       </c>
       <c r="D5" s="15" t="n">
-        <v>0.1333206794668913</v>
+        <v>0.02161189738565117</v>
       </c>
       <c r="E5" s="15" t="n">
-        <v>-0.03193410589144496</v>
+        <v>-0.02115470409160025</v>
       </c>
       <c r="F5" s="15" t="n">
-        <v>0.006979366637694051</v>
+        <v>-0.03108467069162479</v>
       </c>
       <c r="G5" s="15" t="n">
-        <v>0.02237399954544061</v>
+        <v>0.02780488916794677</v>
       </c>
       <c r="H5" s="15" t="n">
-        <v>-0.03391883289898012</v>
+        <v>-0.007432534602163088</v>
       </c>
       <c r="I5" s="15" t="n">
-        <v>0.02310455120636323</v>
+        <v>-0.01227990172828619</v>
       </c>
       <c r="J5" s="15" t="n">
-        <v>-0.01363087020111209</v>
+        <v>0.005155646224368482</v>
       </c>
       <c r="K5" s="15" t="n">
-        <v>0.003255030407142812</v>
+        <v>-0.006335290627493939</v>
       </c>
       <c r="L5" s="15" t="n">
-        <v>0.007664267572485173</v>
+        <v>-0.006679384401248822</v>
       </c>
       <c r="M5" s="15" t="n">
-        <v>-0.07217108571541242</v>
+        <v>0.04340116016951634</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="15" t="n">
-        <v>2017</v>
+        <v>2020</v>
       </c>
       <c r="B6" s="15" t="n">
-        <v>-0.0268533167902304</v>
+        <v>-0.01347524423010971</v>
       </c>
       <c r="C6" s="15" t="n">
-        <v>0.01529326809540343</v>
+        <v>-0.002078196157955126</v>
       </c>
       <c r="D6" s="15" t="n">
-        <v>-0.007295269279153915</v>
+        <v>-0.01785280066188777</v>
       </c>
       <c r="E6" s="15" t="n">
-        <v>-0.02098525934851525</v>
+        <v>0.006059105557672417</v>
       </c>
       <c r="F6" s="15" t="n">
-        <v>-0.03294739152649595</v>
+        <v>-0.01204522780858819</v>
       </c>
       <c r="G6" s="15" t="n">
-        <v>0.02250870249392056</v>
+        <v>0.03200473792083436</v>
       </c>
       <c r="H6" s="15" t="n">
-        <v>-0.03241612775806446</v>
+        <v>0.06881573755255399</v>
       </c>
       <c r="I6" s="15" t="n">
-        <v>0.04633136896066259</v>
+        <v>0.005803095796527824</v>
       </c>
       <c r="J6" s="15" t="n">
-        <v>0.006893387645152016</v>
+        <v>-0.01593468122252883</v>
       </c>
       <c r="K6" s="15" t="n">
-        <v>0.001753979850733334</v>
+        <v>-0.01647198938158267</v>
       </c>
       <c r="L6" s="15" t="n">
-        <v>-0.03744588349195299</v>
+        <v>0.02072233628747933</v>
       </c>
       <c r="M6" s="15" t="n">
-        <v>-0.006804970669783916</v>
+        <v>-6.661338147750939e-16</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="15" t="n">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="B7" s="15" t="n">
-        <v>-0.007167830414052778</v>
+        <v>-0.01835521644047988</v>
       </c>
       <c r="C7" s="15" t="n">
-        <v>0.007619891684661706</v>
+        <v>-0.01643125512155807</v>
       </c>
       <c r="D7" s="15" t="n">
-        <v>0.05980193991728666</v>
+        <v>-0.01757014530604928</v>
       </c>
       <c r="E7" s="15" t="n">
-        <v>-0.0364590162161722</v>
+        <v>-0.001758711537505731</v>
       </c>
       <c r="F7" s="15" t="n">
-        <v>-0.02466598582579071</v>
+        <v>0.03318756156126801</v>
       </c>
       <c r="G7" s="15" t="n">
-        <v>-0.05510688312254941</v>
+        <v>-0.009948872377588458</v>
       </c>
       <c r="H7" s="15" t="n">
-        <v>-0.02041462481518042</v>
+        <v>-0.02325712722340845</v>
       </c>
       <c r="I7" s="15" t="n">
-        <v>-0.05779163869620385</v>
+        <v>0.02998417059079173</v>
       </c>
       <c r="J7" s="15" t="n">
-        <v>-0.0112097898061333</v>
+        <v>0.007705588826218746</v>
       </c>
       <c r="K7" s="15" t="n">
-        <v>-0.06922159137661477</v>
+        <v>-0.01331107777472618</v>
       </c>
       <c r="L7" s="15" t="n">
-        <v>0.03087736442434008</v>
+        <v>-0.0005742774324535294</v>
       </c>
       <c r="M7" s="15" t="n">
-        <v>-0.04389477075404769</v>
+        <v>0.01952983478575843</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="15" t="n">
-        <v>2019</v>
+        <v>2022</v>
       </c>
       <c r="B8" s="15" t="n">
-        <v>-0.01312059982655389</v>
+        <v>-0.02817046714830651</v>
       </c>
       <c r="C8" s="15" t="n">
-        <v>0.1798293690782575</v>
+        <v>-0.0165223212047757</v>
       </c>
       <c r="D8" s="15" t="n">
-        <v>0.07608889138724173</v>
+        <v>-0.0182740954402717</v>
       </c>
       <c r="E8" s="15" t="n">
-        <v>-0.0292703147302501</v>
+        <v>-0.02341747280246109</v>
       </c>
       <c r="F8" s="15" t="n">
-        <v>-0.06075274871470859</v>
+        <v>0.001536607537508061</v>
       </c>
       <c r="G8" s="15" t="n">
-        <v>0.01509168912011694</v>
+        <v>0.028239984178698</v>
       </c>
       <c r="H8" s="15" t="n">
-        <v>0.02896482234529252</v>
+        <v>-0.003881112828626687</v>
       </c>
       <c r="I8" s="15" t="n">
-        <v>0.01860802221768454</v>
+        <v/>
       </c>
       <c r="J8" s="15" t="n">
-        <v>0.007507782274812635</v>
+        <v/>
       </c>
       <c r="K8" s="15" t="n">
-        <v>0.01959193814041194</v>
+        <v/>
       </c>
       <c r="L8" s="15" t="n">
-        <v>-0.002816767411122467</v>
+        <v/>
       </c>
       <c r="M8" s="15" t="n">
-        <v>0.05806139138223054</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="15" t="n">
-        <v>2020</v>
-      </c>
-      <c r="B9" s="15" t="n">
-        <v>0.05232883657313869</v>
-      </c>
-      <c r="C9" s="15" t="n">
-        <v>0.05421785507717791</v>
-      </c>
-      <c r="D9" s="15" t="n">
-        <v>-0.06890229742058573</v>
-      </c>
-      <c r="E9" s="15" t="n">
-        <v>0.07505581786251803</v>
-      </c>
-      <c r="F9" s="15" t="n">
-        <v>0.006463752937315936</v>
-      </c>
-      <c r="G9" s="15" t="n">
-        <v>0.1192189744666308</v>
-      </c>
-      <c r="H9" s="15" t="n">
-        <v>0.1053531872230831</v>
-      </c>
-      <c r="I9" s="15" t="n">
-        <v>-0.01723002064248569</v>
-      </c>
-      <c r="J9" s="15" t="n">
-        <v>-0.03978815493142718</v>
-      </c>
-      <c r="K9" s="15" t="n">
-        <v>0.02264057540035869</v>
-      </c>
-      <c r="L9" s="15" t="n">
-        <v>-0.006544362266877934</v>
-      </c>
-      <c r="M9" s="15" t="n">
-        <v>0.09136600612623558</v>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -1738,7 +1677,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
@@ -1816,330 +1755,289 @@
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" s="15" t="n">
-        <v>2013</v>
+        <v>2016</v>
       </c>
       <c r="B2" s="15" t="n">
-        <v>-0.007785255783889111</v>
+        <v/>
       </c>
       <c r="C2" s="15" t="n">
-        <v>-0.01959380757657325</v>
+        <v/>
       </c>
       <c r="D2" s="15" t="n">
-        <v>-0.002707575914357441</v>
+        <v/>
       </c>
       <c r="E2" s="15" t="n">
-        <v>-0.006888929464910265</v>
+        <v/>
       </c>
       <c r="F2" s="15" t="n">
-        <v>-0.04302326037705495</v>
+        <v/>
       </c>
       <c r="G2" s="15" t="n">
-        <v>0.01241580651633822</v>
+        <v/>
       </c>
       <c r="H2" s="15" t="n">
-        <v>-0.0306639228514024</v>
+        <v/>
       </c>
       <c r="I2" s="15" t="n">
-        <v>-0.01409439793184775</v>
+        <v/>
       </c>
       <c r="J2" s="15" t="n">
-        <v>-0.03918993831393947</v>
+        <v>-0.001779911150208813</v>
       </c>
       <c r="K2" s="15" t="n">
-        <v>0.02635797329400602</v>
+        <v>0.006962824991982863</v>
       </c>
       <c r="L2" s="15" t="n">
-        <v>-0.02916380432750043</v>
+        <v>0.008400970834451904</v>
       </c>
       <c r="M2" s="15" t="n">
-        <v>0.009573954246379524</v>
+        <v>0.07618618381100339</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="15" t="n">
-        <v>2014</v>
+        <v>2017</v>
       </c>
       <c r="B3" s="15" t="n">
-        <v>-0.0387653612216351</v>
+        <v>0.04127807877097545</v>
       </c>
       <c r="C3" s="15" t="n">
-        <v>0.009767305960752815</v>
+        <v>-0.01875162763877591</v>
       </c>
       <c r="D3" s="15" t="n">
-        <v>0.02110426001157761</v>
+        <v>-0.001422661504436595</v>
       </c>
       <c r="E3" s="15" t="n">
-        <v>0.01011729128052319</v>
+        <v>0.02385912896452291</v>
       </c>
       <c r="F3" s="15" t="n">
-        <v>-0.008685520763640819</v>
+        <v>0.04484144384905653</v>
       </c>
       <c r="G3" s="15" t="n">
-        <v>-0.01810475884383977</v>
+        <v>-0.02537208060393192</v>
       </c>
       <c r="H3" s="15" t="n">
-        <v>0.013954703332129</v>
+        <v>0.05600736976686482</v>
       </c>
       <c r="I3" s="15" t="n">
-        <v>-0.01601770996950769</v>
+        <v>-0.04251490369857025</v>
       </c>
       <c r="J3" s="15" t="n">
-        <v>-0.02252510264670593</v>
+        <v>-0.01509693099575349</v>
       </c>
       <c r="K3" s="15" t="n">
-        <v>0.004482874019154259</v>
+        <v>-0.02521264593596062</v>
       </c>
       <c r="L3" s="15" t="n">
-        <v>-0.01115599561519343</v>
+        <v>0.05416285970856061</v>
       </c>
       <c r="M3" s="15" t="n">
-        <v>0.01706406083238599</v>
+        <v>-0.01719115492605661</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="15" t="n">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="B4" s="15" t="n">
-        <v>-0.04080736878085378</v>
+        <v>0.02852150430777467</v>
       </c>
       <c r="C4" s="15" t="n">
-        <v>-0.03986083812911145</v>
+        <v>-0.05052959178541627</v>
       </c>
       <c r="D4" s="15" t="n">
-        <v>-0.05711859941025321</v>
+        <v>-0.08924792460936704</v>
       </c>
       <c r="E4" s="15" t="n">
-        <v>-0.06120820217318101</v>
+        <v>0.04504754495799634</v>
       </c>
       <c r="F4" s="15" t="n">
-        <v>-0.06472687981636938</v>
+        <v>0.01737907413672835</v>
       </c>
       <c r="G4" s="15" t="n">
-        <v>0.0576471818178681</v>
+        <v>0.05168334779644113</v>
       </c>
       <c r="H4" s="15" t="n">
-        <v>0.02876694567852334</v>
+        <v>0.02513587204386658</v>
       </c>
       <c r="I4" s="15" t="n">
-        <v>0.06696783802668915</v>
+        <v>0.06874597802861815</v>
       </c>
       <c r="J4" s="15" t="n">
-        <v>-0.02010489743897159</v>
+        <v>0.01858227600675511</v>
       </c>
       <c r="K4" s="15" t="n">
-        <v>-0.05321392437921368</v>
+        <v>0.104461365513419</v>
       </c>
       <c r="L4" s="15" t="n">
-        <v>-0.02576242860676636</v>
+        <v>-0.04071269010317835</v>
       </c>
       <c r="M4" s="15" t="n">
-        <v>-0.0062088454393735</v>
+        <v>0.04244949090683803</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="15" t="n">
-        <v>2016</v>
+        <v>2019</v>
       </c>
       <c r="B5" s="15" t="n">
-        <v>0.0877643206727623</v>
+        <v>0.03451999042020737</v>
       </c>
       <c r="C5" s="15" t="n">
-        <v>0.01539499542242528</v>
+        <v>-0.1464309906086505</v>
       </c>
       <c r="D5" s="15" t="n">
-        <v>-0.05280958320903617</v>
+        <v>-0.08158771286270405</v>
       </c>
       <c r="E5" s="15" t="n">
-        <v>0.01104848315070051</v>
+        <v>0.01677045544741551</v>
       </c>
       <c r="F5" s="15" t="n">
-        <v>-0.005487458264680778</v>
+        <v>0.05079420367073118</v>
       </c>
       <c r="G5" s="15" t="n">
-        <v>-0.01094004634879664</v>
+        <v>0.005921671489687252</v>
       </c>
       <c r="H5" s="15" t="n">
-        <v>0.01271302722274736</v>
+        <v>-0.0477399338123129</v>
       </c>
       <c r="I5" s="15" t="n">
-        <v>-0.009987347243134104</v>
+        <v>-0.03924524206125524</v>
       </c>
       <c r="J5" s="15" t="n">
-        <v>0.005079754792204572</v>
+        <v>-0.008138029786882939</v>
       </c>
       <c r="K5" s="15" t="n">
-        <v>-0.001726877213826472</v>
+        <v>-0.03383210721375474</v>
       </c>
       <c r="L5" s="15" t="n">
-        <v>-0.003463828973343297</v>
+        <v>-0.004985846962344609</v>
       </c>
       <c r="M5" s="15" t="n">
-        <v>0.03100919068427488</v>
+        <v>-0.03566021923462925</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="15" t="n">
-        <v>2017</v>
+        <v>2020</v>
       </c>
       <c r="B6" s="15" t="n">
-        <v>0.01128471945798748</v>
+        <v>-0.08273744800837912</v>
       </c>
       <c r="C6" s="15" t="n">
-        <v>-0.006510010140763023</v>
+        <v>-0.08428122418785644</v>
       </c>
       <c r="D6" s="15" t="n">
-        <v>0.002604669568400109</v>
+        <v>0.07571494187622241</v>
       </c>
       <c r="E6" s="15" t="n">
-        <v>0.008458558923076787</v>
+        <v>-0.09367590231187961</v>
       </c>
       <c r="F6" s="15" t="n">
-        <v>0.01418845599181906</v>
+        <v>-0.02320021656120463</v>
       </c>
       <c r="G6" s="15" t="n">
-        <v>-0.008570041464913691</v>
+        <v>-0.1190029972728179</v>
       </c>
       <c r="H6" s="15" t="n">
-        <v>0.01165396082407333</v>
+        <v>-0.0778422109554382</v>
       </c>
       <c r="I6" s="15" t="n">
-        <v>-0.01829587438282765</v>
+        <v>0.02569933014110348</v>
       </c>
       <c r="J6" s="15" t="n">
-        <v>-0.002875894614183028</v>
+        <v>0.03720292035012873</v>
       </c>
       <c r="K6" s="15" t="n">
-        <v>-0.0003119003665547071</v>
+        <v>-0.05052619537136849</v>
       </c>
       <c r="L6" s="15" t="n">
-        <v>0.01565075547748651</v>
+        <v>0.02616946181878221</v>
       </c>
       <c r="M6" s="15" t="n">
-        <v>0.002569042547400535</v>
+        <v>-0.116169711064516</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="15" t="n">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="B7" s="15" t="n">
-        <v>0.0018702877132033</v>
+        <v>-0.07616162325274167</v>
       </c>
       <c r="C7" s="15" t="n">
-        <v>-0.005339461597297257</v>
+        <v>0.0496510951033915</v>
       </c>
       <c r="D7" s="15" t="n">
-        <v>-0.02462949798414182</v>
+        <v>0.02617216231205854</v>
       </c>
       <c r="E7" s="15" t="n">
-        <v>0.01293850215596137</v>
+        <v>-0.1131208834469581</v>
       </c>
       <c r="F7" s="15" t="n">
-        <v>0.009033495279918036</v>
+        <v>-0.03883771778645517</v>
       </c>
       <c r="G7" s="15" t="n">
-        <v>0.02277566780702944</v>
+        <v>-0.06239397103287569</v>
       </c>
       <c r="H7" s="15" t="n">
-        <v>0.006737027902571135</v>
+        <v>-0.0233639371066906</v>
       </c>
       <c r="I7" s="15" t="n">
-        <v>0.02268392974625066</v>
+        <v>0.09699698894085595</v>
       </c>
       <c r="J7" s="15" t="n">
-        <v>0.004696775882413684</v>
+        <v>-0.005831449518900356</v>
       </c>
       <c r="K7" s="15" t="n">
-        <v>0.02633477462625722</v>
+        <v>-0.04633227685541652</v>
       </c>
       <c r="L7" s="15" t="n">
-        <v>-0.0127302280899827</v>
+        <v>-0.0432674250036339</v>
       </c>
       <c r="M7" s="15" t="n">
-        <v>0.01540236427224095</v>
+        <v>0.06942497670727099</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="15" t="n">
-        <v>2019</v>
+        <v>2022</v>
       </c>
       <c r="B8" s="15" t="n">
-        <v>0.004178575836472742</v>
+        <v>0.1046145229712754</v>
       </c>
       <c r="C8" s="15" t="n">
-        <v>-0.05878770853270776</v>
+        <v>-0.01193153720842532</v>
       </c>
       <c r="D8" s="15" t="n">
-        <v>-0.02754757853415934</v>
+        <v>0.05315697488611626</v>
       </c>
       <c r="E8" s="15" t="n">
-        <v>0.01079144343876481</v>
+        <v>0.1068478851536141</v>
       </c>
       <c r="F8" s="15" t="n">
-        <v>0.02390536730023074</v>
+        <v>-0.03819164736497982</v>
       </c>
       <c r="G8" s="15" t="n">
-        <v>-0.004731811937227492</v>
+        <v>-0.1253646308965031</v>
       </c>
       <c r="H8" s="15" t="n">
-        <v>-0.01068938860872015</v>
+        <v>0.006315318105666989</v>
       </c>
       <c r="I8" s="15" t="n">
-        <v>-0.00797594770891874</v>
+        <v/>
       </c>
       <c r="J8" s="15" t="n">
-        <v>-0.003835122360847265</v>
+        <v/>
       </c>
       <c r="K8" s="15" t="n">
-        <v>-0.007627793841263997</v>
+        <v/>
       </c>
       <c r="L8" s="15" t="n">
-        <v>0.0003767206664748723</v>
+        <v/>
       </c>
       <c r="M8" s="15" t="n">
-        <v>-0.02109044108452818</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="15" t="n">
-        <v>2020</v>
-      </c>
-      <c r="B9" s="15" t="n">
-        <v>-0.01955683538121766</v>
-      </c>
-      <c r="C9" s="15" t="n">
-        <v>-0.02422600384061724</v>
-      </c>
-      <c r="D9" s="15" t="n">
-        <v>0.0261370982970881</v>
-      </c>
-      <c r="E9" s="15" t="n">
-        <v>-0.02897296139733085</v>
-      </c>
-      <c r="F9" s="15" t="n">
-        <v>-0.002841577138439466</v>
-      </c>
-      <c r="G9" s="15" t="n">
-        <v>-0.04312229904678622</v>
-      </c>
-      <c r="H9" s="15" t="n">
-        <v>-0.04018846857540714</v>
-      </c>
-      <c r="I9" s="15" t="n">
-        <v>0.005113516196288304</v>
-      </c>
-      <c r="J9" s="15" t="n">
-        <v>0.01553720503731393</v>
-      </c>
-      <c r="K9" s="15" t="n">
-        <v>-0.01003750697531414</v>
-      </c>
-      <c r="L9" s="15" t="n">
-        <v>0.001217359128621087</v>
-      </c>
-      <c r="M9" s="15" t="n">
-        <v>-0.03311781605890063</v>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>